<commit_message>
Icons added.  Rendering becoming intelligent
</commit_message>
<xml_diff>
--- a/fullCalendarWorking/shsCalendarFeatures.xlsx
+++ b/fullCalendarWorking/shsCalendarFeatures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mrsw.shs\mrsw.shs\fullCalendarWorking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mrsw.shs\fullCalendarWorking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Feature</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Pre-req</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -182,9 +185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -525,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -537,7 +541,7 @@
     <col min="3" max="3" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -547,8 +551,11 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -556,7 +563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -564,15 +571,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>42153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -580,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -591,7 +601,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -599,7 +609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -610,7 +620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -618,7 +628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -629,7 +639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -640,7 +650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -651,7 +661,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -659,7 +669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -667,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -675,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>

</xml_diff>